<commit_message>
ders-17 ddt ile farklı senaryo türleri
</commit_message>
<xml_diff>
--- a/testdata/arama.xlsx
+++ b/testdata/arama.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tom/PycharmProjects/pytest-selenium-framework/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23FEEC36-779F-844A-A6BB-E38EF24C24AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91AC758E-1823-BD41-8814-1C8CBFD9AC11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16200" xr2:uid="{C986B587-095D-0D4E-B3AE-52978ABB8AF0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>kelime</t>
   </si>
@@ -51,6 +51,18 @@
   </si>
   <si>
     <t>No products were found that matched your criteria.</t>
+  </si>
+  <si>
+    <t>senaryoturu</t>
+  </si>
+  <si>
+    <t>negatif</t>
+  </si>
+  <si>
+    <t>pozitif</t>
+  </si>
+  <si>
+    <t>diamond</t>
   </si>
 </sst>
 </file>
@@ -409,39 +421,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43C7F1D4-0261-4E4A-AF09-75113AF4A3B8}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="2" max="2" width="46.5" customWidth="1"/>
+    <col min="3" max="3" width="46.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>